<commit_message>
Update to include pre-defined coeficients
</commit_message>
<xml_diff>
--- a/LGSpeakers/Settings.xlsx
+++ b/LGSpeakers/Settings.xlsx
@@ -13,6 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Bass Boost" sheetId="3" r:id="rId3"/>
+    <sheet name="Power on" sheetId="4" r:id="rId4"/>
+    <sheet name="Standard" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="88">
   <si>
     <t>Add</t>
   </si>
@@ -210,6 +214,84 @@
   </si>
   <si>
     <t>Default values</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>6088b7</t>
+  </si>
+  <si>
+    <t>bf7628</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>1f28</t>
+  </si>
+  <si>
+    <t>1f0e</t>
+  </si>
+  <si>
+    <t>c0,33,9f,1f,c2,01,3f,cc,61,e0,33,65,20,0a,99</t>
+  </si>
+  <si>
+    <t>1f0f</t>
+  </si>
+  <si>
+    <t>c0,26,41,1f,ec,df,3f,d9,b4,e0,26,35,1f,ec,df</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>0,0,0,0,0,0,0,0,0,0,0,0,20,0,0</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>1e</t>
+  </si>
+  <si>
+    <t>Power on</t>
+  </si>
+  <si>
+    <t>Power off</t>
+  </si>
+  <si>
+    <t>1f30</t>
+  </si>
+  <si>
+    <t>c0,b1,23,1f,4f,36,3f,4e,dd,e0,b0,ca,20,00,00</t>
+  </si>
+  <si>
+    <t>c0,26,41,1f,ec,df,3f,d9,4b,e0,26,35,1f,ec,df</t>
+  </si>
+  <si>
+    <t>c0,32,d0,1f,ca,76,3f,cd,30,e0,32,76,20,03,14</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>Standard</t>
   </si>
 </sst>
 </file>
@@ -320,13 +402,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
@@ -613,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +889,7 @@
       <c r="C10" s="1">
         <v>15</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -916,7 +999,7 @@
         <v>35</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" ref="G12:G14" si="6">SUM((R12+N12+O12)/(1+(-P12)+(-Q12)))</f>
+        <f t="shared" ref="G12:G13" si="6">SUM((R12+N12+O12)/(1+(-P12)+(-Q12)))</f>
         <v>0</v>
       </c>
       <c r="H12" s="3">
@@ -935,23 +1018,23 @@
         <v>0</v>
       </c>
       <c r="N12" s="3">
-        <f t="shared" ref="N12:N14" si="7">HEX2DEC(H12)</f>
+        <f t="shared" ref="N12:N13" si="7">HEX2DEC(H12)</f>
         <v>0</v>
       </c>
       <c r="O12" s="3">
-        <f t="shared" ref="O12:O14" si="8">HEX2DEC(I12)</f>
+        <f t="shared" ref="O12:O13" si="8">HEX2DEC(I12)</f>
         <v>0</v>
       </c>
       <c r="P12" s="3">
-        <f t="shared" ref="P12:P14" si="9">HEX2DEC(J12)</f>
+        <f t="shared" ref="P12:P13" si="9">HEX2DEC(J12)</f>
         <v>118</v>
       </c>
       <c r="Q12" s="3">
-        <f t="shared" ref="Q12:Q14" si="10">HEX2DEC(K12)</f>
+        <f t="shared" ref="Q12:Q13" si="10">HEX2DEC(K12)</f>
         <v>136</v>
       </c>
       <c r="R12" s="3">
-        <f t="shared" ref="R12:R14" si="11">HEX2DEC(L12)</f>
+        <f t="shared" ref="R12:R13" si="11">HEX2DEC(L12)</f>
         <v>0</v>
       </c>
     </row>
@@ -1485,4 +1568,910 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f>SUM((L2+H2+I2)/(1+(-J2)+(-K2)))</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1">
+        <f>HEX2DEC(B2)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:L5" si="0">HEX2DEC(C2)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f>SUM((L3+H3+I3)/(1+(-J3)+(-K3)))</f>
+        <v>255</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <f>HEX2DEC(B3)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3" si="1">HEX2DEC(C3)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3" si="2">HEX2DEC(D3)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3" si="3">HEX2DEC(E3)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3" si="4">HEX2DEC(F3)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J23" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" t="s">
+        <v>66</v>
+      </c>
+      <c r="L23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f>SUM((L25+H25+I25)/(1+(-J25)+(-K25)))</f>
+        <v>-1.5259023513625408E-5</v>
+      </c>
+      <c r="B25" s="1">
+        <v>90</v>
+      </c>
+      <c r="C25" s="1">
+        <v>48</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="1">
+        <v>48</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <f>HEX2DEC(B25)</f>
+        <v>144</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" ref="I25:L28" si="5">HEX2DEC(C25)</f>
+        <v>72</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="5"/>
+        <v>4159016</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="5"/>
+        <v>14715063</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f>SUM((L26+H26+I26)/(1+J26+K26))</f>
+        <v>1.5259021896696422E-5</v>
+      </c>
+      <c r="B26" s="1">
+        <v>90</v>
+      </c>
+      <c r="C26" s="1">
+        <v>48</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="1">
+        <v>48</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <f t="shared" ref="H26:H28" si="6">HEX2DEC(B26)</f>
+        <v>144</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="5"/>
+        <v>12547624</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="5"/>
+        <v>6326455</v>
+      </c>
+      <c r="L26" s="1">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <f t="shared" ref="A27:A28" si="7">SUM((L27+H27+I27)/(1+(-J27)+(-K27)))</f>
+        <v>0</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>76</v>
+      </c>
+      <c r="E27" s="3">
+        <v>88</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
+        <f t="shared" si="5"/>
+        <v>118</v>
+      </c>
+      <c r="K27" s="3">
+        <f t="shared" si="5"/>
+        <v>136</v>
+      </c>
+      <c r="L27" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <f t="shared" si="7"/>
+        <v>-1.2972972972972974</v>
+      </c>
+      <c r="B28" s="3">
+        <v>90</v>
+      </c>
+      <c r="C28" s="3">
+        <v>48</v>
+      </c>
+      <c r="D28" s="3">
+        <v>28</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="3">
+        <v>48</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3">
+        <f t="shared" si="6"/>
+        <v>144</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="5"/>
+        <v>183</v>
+      </c>
+      <c r="L28" s="3">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>